<commit_message>
Clean up codes and added figures
</commit_message>
<xml_diff>
--- a/Microscopy/FISHMicroscopyResults.xlsx
+++ b/Microscopy/FISHMicroscopyResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ea521192/Desktop/zebrafish-conv-mix9-models/Microscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B78426F-5211-A743-8C63-B7DADF34E716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60253373-BC58-4340-8DA7-982B3780C6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16020" xr2:uid="{37CB6385-C1F7-154B-AC74-102E0513E05A}"/>
+    <workbookView xWindow="360" yWindow="1980" windowWidth="27640" windowHeight="16020" xr2:uid="{37CB6385-C1F7-154B-AC74-102E0513E05A}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -47,9 +47,6 @@
     <t>FishNumSlide</t>
   </si>
   <si>
-    <t>StrainCondition</t>
-  </si>
-  <si>
     <t>DateImaged</t>
   </si>
   <si>
@@ -122,15 +119,6 @@
     <t>TotalIntestineArea</t>
   </si>
   <si>
-    <t>NormalizedIntestineMucus</t>
-  </si>
-  <si>
-    <t>Bacteria vs Mucus</t>
-  </si>
-  <si>
-    <t>Conventional</t>
-  </si>
-  <si>
     <t>Eub338-AF594</t>
   </si>
   <si>
@@ -336,6 +324,15 @@
   </si>
   <si>
     <t>Eub338-AF627</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Conv</t>
+  </si>
+  <si>
+    <t>BacteriavsMucus</t>
   </si>
 </sst>
 </file>
@@ -411,13 +408,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419460</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -666,13 +663,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419460</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1955,10 +1952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7849A8-1A3E-5D41-8C41-1353ADE06461}">
-  <dimension ref="A1:AD35"/>
+  <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD41" sqref="AD41"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1971,17 +1968,18 @@
     <col min="14" max="14" width="12.83203125" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.1640625" style="3" customWidth="1"/>
     <col min="16" max="16" width="15.1640625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="17.5" style="3" customWidth="1"/>
-    <col min="18" max="18" width="17.83203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="19.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="21" style="3" customWidth="1"/>
     <col min="19" max="19" width="19.5" style="3" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" style="3" customWidth="1"/>
     <col min="21" max="21" width="19.33203125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="19.1640625" style="3" customWidth="1"/>
     <col min="23" max="24" width="16.83203125" style="3" customWidth="1"/>
     <col min="25" max="25" width="19.33203125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="10.6640625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="13.5" style="3" customWidth="1"/>
-    <col min="28" max="29" width="13" style="3" customWidth="1"/>
+    <col min="26" max="26" width="20" style="3" customWidth="1"/>
+    <col min="27" max="27" width="18.5" style="3" customWidth="1"/>
+    <col min="28" max="28" width="16.33203125" style="3" customWidth="1"/>
+    <col min="30" max="30" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -1995,86 +1993,84 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="AC1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="AD1"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A2">
@@ -2087,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E2">
         <v>20220524</v>
@@ -2096,25 +2092,25 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J2">
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N2" s="3">
         <v>84900</v>
@@ -2126,7 +2122,7 @@
         <v>135000</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:Q11" si="0">O2/P2</f>
+        <f>O2/P2</f>
         <v>236.2962962962963</v>
       </c>
       <c r="R2" s="3">
@@ -2136,7 +2132,7 @@
         <v>32900</v>
       </c>
       <c r="T2" s="3">
-        <f t="shared" ref="T2:T11" si="1">R2/S2</f>
+        <f t="shared" ref="T2:T11" si="0">R2/S2</f>
         <v>434.65045592705167</v>
       </c>
       <c r="U2" s="3">
@@ -2149,14 +2145,14 @@
         <v>11500</v>
       </c>
       <c r="X2" s="3">
-        <f t="shared" ref="X2:X11" si="2">V2/W2</f>
+        <f t="shared" ref="X2:X11" si="1">V2/W2</f>
         <v>94.782608695652172</v>
       </c>
       <c r="Y2" s="3">
         <v>33.6</v>
       </c>
       <c r="Z2" s="3">
-        <f t="shared" ref="Z2:Z11" si="3">N2+U2+Y2</f>
+        <f t="shared" ref="Z2:Z11" si="2">N2+U2+Y2</f>
         <v>168033.6</v>
       </c>
       <c r="AA2" s="3">
@@ -2168,13 +2164,10 @@
         <v>44400</v>
       </c>
       <c r="AC2" s="3">
-        <f t="shared" ref="AC2:AC11" si="4">AA2/AB2</f>
-        <v>346.62162162162161</v>
-      </c>
-      <c r="AD2" s="3">
         <f>Z2/Q2</f>
         <v>711.11398119122259</v>
       </c>
+      <c r="AD2" s="3"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A3">
@@ -2187,7 +2180,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E3">
         <v>20220524</v>
@@ -2196,25 +2189,25 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J3">
         <v>100</v>
       </c>
       <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
         <v>34</v>
       </c>
-      <c r="L3" t="s">
-        <v>38</v>
-      </c>
       <c r="M3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
@@ -2226,7 +2219,7 @@
         <v>116500</v>
       </c>
       <c r="Q3" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q2:Q11" si="3">O3/P3</f>
         <v>205.15021459227466</v>
       </c>
       <c r="R3" s="3">
@@ -2236,7 +2229,7 @@
         <v>26500</v>
       </c>
       <c r="T3" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>352.07547169811323</v>
       </c>
       <c r="U3" s="3">
@@ -2249,30 +2242,26 @@
         <v>9675</v>
       </c>
       <c r="X3" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>196.38242894056847</v>
       </c>
       <c r="Y3" s="3">
         <v>637</v>
       </c>
       <c r="Z3" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1022</v>
       </c>
       <c r="AA3" s="3">
-        <f t="shared" ref="AA3:AB35" si="5">R3+V3</f>
+        <f t="shared" ref="AA3:AB31" si="4">R3+V3</f>
         <v>11230000</v>
       </c>
       <c r="AB3" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>36175</v>
       </c>
       <c r="AC3" s="3">
-        <f t="shared" si="4"/>
-        <v>310.43538355217692</v>
-      </c>
-      <c r="AD3" s="3">
-        <f t="shared" ref="AD3:AD23" si="6">Z3/Q3</f>
+        <f t="shared" ref="AC3:AC21" si="5">Z3/Q3</f>
         <v>4.9817154811715483</v>
       </c>
     </row>
@@ -2287,7 +2276,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E4">
         <v>20220613</v>
@@ -2296,25 +2285,25 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J4">
         <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N4" s="3">
         <v>279000</v>
@@ -2326,7 +2315,7 @@
         <v>130000</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>357.69230769230768</v>
       </c>
       <c r="R4" s="3">
@@ -2336,7 +2325,7 @@
         <v>33700</v>
       </c>
       <c r="T4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>445.10385756676556</v>
       </c>
       <c r="U4" s="3">
@@ -2349,30 +2338,26 @@
         <v>16500</v>
       </c>
       <c r="X4" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>557.57575757575762</v>
       </c>
       <c r="Y4" s="3">
         <v>1253</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>368553</v>
       </c>
       <c r="AA4" s="3">
+        <f t="shared" si="4"/>
+        <v>24200000</v>
+      </c>
+      <c r="AB4" s="3">
+        <f t="shared" si="4"/>
+        <v>50200</v>
+      </c>
+      <c r="AC4" s="3">
         <f t="shared" si="5"/>
-        <v>24200000</v>
-      </c>
-      <c r="AB4" s="3">
-        <f t="shared" si="5"/>
-        <v>50200</v>
-      </c>
-      <c r="AC4" s="3">
-        <f t="shared" si="4"/>
-        <v>482.07171314741038</v>
-      </c>
-      <c r="AD4" s="3">
-        <f t="shared" si="6"/>
         <v>1030.3632258064517</v>
       </c>
     </row>
@@ -2387,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E5">
         <v>20220520</v>
@@ -2396,25 +2381,25 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J5">
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="N5" s="3">
         <v>18300</v>
@@ -2426,7 +2411,7 @@
         <v>104000</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>225.96153846153845</v>
       </c>
       <c r="R5" s="3">
@@ -2436,7 +2421,7 @@
         <v>30300</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>249.17491749174917</v>
       </c>
       <c r="U5" s="3">
@@ -2449,30 +2434,26 @@
         <v>25800</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>191.47286821705427</v>
       </c>
       <c r="Y5" s="3">
         <v>862</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>114762</v>
       </c>
       <c r="AA5" s="3">
+        <f t="shared" si="4"/>
+        <v>12490000</v>
+      </c>
+      <c r="AB5" s="3">
+        <f t="shared" si="4"/>
+        <v>56100</v>
+      </c>
+      <c r="AC5" s="3">
         <f t="shared" si="5"/>
-        <v>12490000</v>
-      </c>
-      <c r="AB5" s="3">
-        <f t="shared" si="5"/>
-        <v>56100</v>
-      </c>
-      <c r="AC5" s="3">
-        <f t="shared" si="4"/>
-        <v>222.63814616755792</v>
-      </c>
-      <c r="AD5" s="3">
-        <f t="shared" si="6"/>
         <v>507.8828936170213</v>
       </c>
     </row>
@@ -2487,7 +2468,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E6">
         <v>20220520</v>
@@ -2496,25 +2477,25 @@
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N6" s="3">
         <v>131000</v>
@@ -2526,7 +2507,7 @@
         <v>116000</v>
       </c>
       <c r="Q6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>140.51724137931035</v>
       </c>
       <c r="R6" s="3">
@@ -2536,7 +2517,7 @@
         <v>30000</v>
       </c>
       <c r="T6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>208.33333333333334</v>
       </c>
       <c r="U6" s="3">
@@ -2549,30 +2530,26 @@
         <v>6748</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>256.37225844694723</v>
       </c>
       <c r="Y6" s="3">
         <v>32</v>
       </c>
       <c r="Z6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>153632</v>
       </c>
       <c r="AA6" s="3">
+        <f t="shared" si="4"/>
+        <v>7980000</v>
+      </c>
+      <c r="AB6" s="3">
+        <f t="shared" si="4"/>
+        <v>36748</v>
+      </c>
+      <c r="AC6" s="3">
         <f t="shared" si="5"/>
-        <v>7980000</v>
-      </c>
-      <c r="AB6" s="3">
-        <f t="shared" si="5"/>
-        <v>36748</v>
-      </c>
-      <c r="AC6" s="3">
-        <f t="shared" si="4"/>
-        <v>217.15467508435833</v>
-      </c>
-      <c r="AD6" s="3">
-        <f t="shared" si="6"/>
         <v>1093.3320245398772</v>
       </c>
     </row>
@@ -2587,7 +2564,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E7">
         <v>20220524</v>
@@ -2596,25 +2573,25 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J7">
         <v>100</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N7" s="3">
         <v>367000</v>
@@ -2626,7 +2603,7 @@
         <v>142000</v>
       </c>
       <c r="Q7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>266.90140845070425</v>
       </c>
       <c r="R7" s="3">
@@ -2636,7 +2613,7 @@
         <v>39200</v>
       </c>
       <c r="T7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>390.30612244897958</v>
       </c>
       <c r="U7" s="3">
@@ -2649,30 +2626,26 @@
         <v>10500</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>548.57142857142856</v>
       </c>
       <c r="Y7" s="3">
         <v>238</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>454438</v>
       </c>
       <c r="AA7" s="3">
+        <f t="shared" si="4"/>
+        <v>21060000</v>
+      </c>
+      <c r="AB7" s="3">
+        <f t="shared" si="4"/>
+        <v>49700</v>
+      </c>
+      <c r="AC7" s="3">
         <f t="shared" si="5"/>
-        <v>21060000</v>
-      </c>
-      <c r="AB7" s="3">
-        <f t="shared" si="5"/>
-        <v>49700</v>
-      </c>
-      <c r="AC7" s="3">
-        <f t="shared" si="4"/>
-        <v>423.74245472837021</v>
-      </c>
-      <c r="AD7" s="3">
-        <f t="shared" si="6"/>
         <v>1702.6436939313983</v>
       </c>
     </row>
@@ -2687,7 +2660,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E8">
         <v>20220524</v>
@@ -2696,25 +2669,25 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J8">
         <v>100</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N8" s="3">
         <v>555000</v>
@@ -2726,7 +2699,7 @@
         <v>133000</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>169.17293233082708</v>
       </c>
       <c r="R8" s="3">
@@ -2736,7 +2709,7 @@
         <v>37400</v>
       </c>
       <c r="T8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>156.14973262032086</v>
       </c>
       <c r="U8" s="3">
@@ -2749,30 +2722,26 @@
         <v>13600</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>639.70588235294122</v>
       </c>
       <c r="Y8" s="3">
         <v>9.4700000000000006</v>
       </c>
       <c r="Z8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>661009.47</v>
       </c>
       <c r="AA8" s="3">
+        <f t="shared" si="4"/>
+        <v>14540000</v>
+      </c>
+      <c r="AB8" s="3">
+        <f t="shared" si="4"/>
+        <v>51000</v>
+      </c>
+      <c r="AC8" s="3">
         <f t="shared" si="5"/>
-        <v>14540000</v>
-      </c>
-      <c r="AB8" s="3">
-        <f t="shared" si="5"/>
-        <v>51000</v>
-      </c>
-      <c r="AC8" s="3">
-        <f t="shared" si="4"/>
-        <v>285.0980392156863</v>
-      </c>
-      <c r="AD8" s="3">
-        <f t="shared" si="6"/>
         <v>3907.3004226666662</v>
       </c>
     </row>
@@ -2787,7 +2756,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E9">
         <v>20220524</v>
@@ -2796,25 +2765,25 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N9" s="3">
         <v>505000</v>
@@ -2826,7 +2795,7 @@
         <v>120000</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>211.66666666666666</v>
       </c>
       <c r="R9" s="3">
@@ -2836,7 +2805,7 @@
         <v>24700</v>
       </c>
       <c r="T9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>126.72064777327935</v>
       </c>
       <c r="U9" s="3">
@@ -2849,30 +2818,26 @@
         <v>13300</v>
       </c>
       <c r="X9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>454.13533834586468</v>
       </c>
       <c r="Y9" s="3">
         <v>808</v>
       </c>
       <c r="Z9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>515187</v>
       </c>
       <c r="AA9" s="3">
+        <f t="shared" si="4"/>
+        <v>9170000</v>
+      </c>
+      <c r="AB9" s="3">
+        <f t="shared" si="4"/>
+        <v>38000</v>
+      </c>
+      <c r="AC9" s="3">
         <f t="shared" si="5"/>
-        <v>9170000</v>
-      </c>
-      <c r="AB9" s="3">
-        <f t="shared" si="5"/>
-        <v>38000</v>
-      </c>
-      <c r="AC9" s="3">
-        <f t="shared" si="4"/>
-        <v>241.31578947368422</v>
-      </c>
-      <c r="AD9" s="3">
-        <f t="shared" si="6"/>
         <v>2433.9543307086615</v>
       </c>
     </row>
@@ -2887,7 +2852,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E10">
         <v>20220601</v>
@@ -2896,25 +2861,25 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="N10" s="3">
         <v>423000</v>
@@ -2926,7 +2891,7 @@
         <v>170000</v>
       </c>
       <c r="Q10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>239.41176470588235</v>
       </c>
       <c r="R10" s="3">
@@ -2936,7 +2901,7 @@
         <v>22500</v>
       </c>
       <c r="T10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>141.77777777777777</v>
       </c>
       <c r="U10" s="3">
@@ -2949,30 +2914,26 @@
         <v>19400</v>
       </c>
       <c r="X10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26.237113402061855</v>
       </c>
       <c r="Y10" s="3">
         <v>15100</v>
       </c>
       <c r="Z10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>487800</v>
       </c>
       <c r="AA10" s="3">
+        <f t="shared" si="4"/>
+        <v>3699000</v>
+      </c>
+      <c r="AB10" s="3">
+        <f t="shared" si="4"/>
+        <v>41900</v>
+      </c>
+      <c r="AC10" s="3">
         <f t="shared" si="5"/>
-        <v>3699000</v>
-      </c>
-      <c r="AB10" s="3">
-        <f t="shared" si="5"/>
-        <v>41900</v>
-      </c>
-      <c r="AC10" s="3">
-        <f t="shared" si="4"/>
-        <v>88.281622911694512</v>
-      </c>
-      <c r="AD10" s="3">
-        <f t="shared" si="6"/>
         <v>2037.4938574938576</v>
       </c>
     </row>
@@ -2987,7 +2948,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="E11">
         <v>20220601</v>
@@ -2996,25 +2957,25 @@
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N11" s="3">
         <v>152000</v>
@@ -3026,7 +2987,7 @@
         <v>97500</v>
       </c>
       <c r="Q11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>237.94871794871796</v>
       </c>
       <c r="R11" s="3">
@@ -3036,7 +2997,7 @@
         <v>32500</v>
       </c>
       <c r="T11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>52.307692307692307</v>
       </c>
       <c r="U11" s="3">
@@ -3049,355 +3010,521 @@
         <v>17900</v>
       </c>
       <c r="X11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>105.58659217877096</v>
       </c>
       <c r="Y11" s="3">
         <v>0</v>
       </c>
       <c r="Z11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>174100</v>
       </c>
       <c r="AA11" s="3">
+        <f t="shared" si="4"/>
+        <v>3590000</v>
+      </c>
+      <c r="AB11" s="3">
+        <f t="shared" si="4"/>
+        <v>50400</v>
+      </c>
+      <c r="AC11" s="3">
         <f t="shared" si="5"/>
-        <v>3590000</v>
-      </c>
-      <c r="AB11" s="3">
-        <f t="shared" si="5"/>
-        <v>50400</v>
-      </c>
-      <c r="AC11" s="3">
-        <f t="shared" si="4"/>
-        <v>71.230158730158735</v>
-      </c>
-      <c r="AD11" s="3">
-        <f t="shared" si="6"/>
         <v>731.67025862068965</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12">
+        <v>20220517</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>9220000</v>
+      </c>
+      <c r="P12" s="3">
+        <v>84700</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" ref="Q12:Q21" si="6">O12/P12</f>
+        <v>108.85478158205431</v>
+      </c>
+      <c r="R12" s="3">
+        <v>3230000</v>
+      </c>
+      <c r="S12" s="3">
+        <v>21000</v>
+      </c>
+      <c r="T12" s="3">
+        <f t="shared" ref="T12:T31" si="7">R12/S12</f>
+        <v>153.8095238095238</v>
+      </c>
+      <c r="U12" s="3">
+        <v>7840</v>
+      </c>
+      <c r="V12" s="3">
+        <v>1590000</v>
+      </c>
+      <c r="W12" s="3">
+        <v>12200</v>
+      </c>
+      <c r="X12" s="3">
+        <f t="shared" ref="X12:X21" si="8">V12/W12</f>
+        <v>130.32786885245901</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>1175</v>
+      </c>
       <c r="Z12" s="3">
-        <f>MEDIAN(Z2:Z11)</f>
-        <v>271326.5</v>
-      </c>
-      <c r="AD12" s="3"/>
+        <f t="shared" ref="Z12:Z21" si="9">N12+U12+Y12</f>
+        <v>9015</v>
+      </c>
+      <c r="AA12" s="3">
+        <f t="shared" si="4"/>
+        <v>4820000</v>
+      </c>
+      <c r="AB12" s="3">
+        <f t="shared" si="4"/>
+        <v>33200</v>
+      </c>
+      <c r="AC12" s="3">
+        <f t="shared" si="5"/>
+        <v>82.816757049891535</v>
+      </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="AD13" s="3"/>
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13">
+        <v>20220518</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M13" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="3">
+        <v>276000</v>
+      </c>
+      <c r="O13" s="3">
+        <v>9640000</v>
+      </c>
+      <c r="P13" s="3">
+        <v>121000</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" si="6"/>
+        <v>79.669421487603302</v>
+      </c>
+      <c r="R13" s="3">
+        <v>1800000</v>
+      </c>
+      <c r="S13" s="3">
+        <v>26500</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" si="7"/>
+        <v>67.924528301886795</v>
+      </c>
+      <c r="U13" s="3">
+        <v>54900</v>
+      </c>
+      <c r="V13" s="3">
+        <v>1490000</v>
+      </c>
+      <c r="W13" s="3">
+        <v>10400</v>
+      </c>
+      <c r="X13" s="3">
+        <f t="shared" si="8"/>
+        <v>143.26923076923077</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>515</v>
+      </c>
+      <c r="Z13" s="3">
+        <f t="shared" si="9"/>
+        <v>331415</v>
+      </c>
+      <c r="AA13" s="3">
+        <f t="shared" si="4"/>
+        <v>3290000</v>
+      </c>
+      <c r="AB13" s="3">
+        <f t="shared" si="4"/>
+        <v>36900</v>
+      </c>
+      <c r="AC13" s="3">
+        <f t="shared" si="5"/>
+        <v>4159.8770746887967</v>
+      </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14">
-        <v>20220517</v>
+        <v>20220518</v>
       </c>
       <c r="F14">
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J14">
         <v>100</v>
       </c>
       <c r="K14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N14" s="3">
         <v>0</v>
       </c>
       <c r="O14" s="3">
-        <v>9220000</v>
+        <v>9800000</v>
       </c>
       <c r="P14" s="3">
-        <v>84700</v>
+        <v>113000</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" ref="Q14:Q23" si="7">O14/P14</f>
-        <v>108.85478158205431</v>
+        <f t="shared" si="6"/>
+        <v>86.725663716814154</v>
       </c>
       <c r="R14" s="3">
-        <v>3230000</v>
+        <v>7050000</v>
       </c>
       <c r="S14" s="3">
-        <v>21000</v>
+        <v>34500</v>
       </c>
       <c r="T14" s="3">
-        <f t="shared" ref="T14:T35" si="8">R14/S14</f>
-        <v>153.8095238095238</v>
+        <f t="shared" si="7"/>
+        <v>204.34782608695653</v>
       </c>
       <c r="U14" s="3">
-        <v>7840</v>
+        <v>22600</v>
       </c>
       <c r="V14" s="3">
-        <v>1590000</v>
+        <v>485000</v>
       </c>
       <c r="W14" s="3">
-        <v>12200</v>
+        <v>14700</v>
       </c>
       <c r="X14" s="3">
-        <f t="shared" ref="X14:X23" si="9">V14/W14</f>
-        <v>130.32786885245901</v>
+        <f t="shared" si="8"/>
+        <v>32.993197278911566</v>
       </c>
       <c r="Y14" s="3">
-        <v>1175</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="3">
-        <f t="shared" ref="Z14:Z23" si="10">N14+U14+Y14</f>
-        <v>9015</v>
+        <f t="shared" si="9"/>
+        <v>22600</v>
       </c>
       <c r="AA14" s="3">
+        <f t="shared" si="4"/>
+        <v>7535000</v>
+      </c>
+      <c r="AB14" s="3">
+        <f t="shared" si="4"/>
+        <v>49200</v>
+      </c>
+      <c r="AC14" s="3">
         <f t="shared" si="5"/>
-        <v>4820000</v>
-      </c>
-      <c r="AB14" s="3">
-        <f t="shared" si="5"/>
-        <v>33200</v>
-      </c>
-      <c r="AC14" s="3">
-        <f t="shared" ref="AC14:AC23" si="11">AA14/AB14</f>
-        <v>145.18072289156626</v>
-      </c>
-      <c r="AD14" s="3">
-        <f t="shared" si="6"/>
-        <v>82.816757049891535</v>
+        <v>260.59183673469391</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E15">
-        <v>20220518</v>
+        <v>20220516</v>
       </c>
       <c r="F15">
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J15">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K15" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="L15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N15" s="3">
-        <v>276000</v>
+        <v>249000</v>
       </c>
       <c r="O15" s="3">
-        <v>9640000</v>
+        <v>10400000</v>
       </c>
       <c r="P15" s="3">
-        <v>121000</v>
+        <v>217000</v>
       </c>
       <c r="Q15" s="3">
+        <f t="shared" si="6"/>
+        <v>47.926267281105993</v>
+      </c>
+      <c r="R15" s="3">
+        <v>1560000</v>
+      </c>
+      <c r="S15" s="3">
+        <v>35200</v>
+      </c>
+      <c r="T15" s="3">
         <f t="shared" si="7"/>
-        <v>79.669421487603302</v>
-      </c>
-      <c r="R15" s="3">
-        <v>1800000</v>
-      </c>
-      <c r="S15" s="3">
-        <v>26500</v>
-      </c>
-      <c r="T15" s="3">
+        <v>44.31818181818182</v>
+      </c>
+      <c r="U15" s="3">
+        <v>31400</v>
+      </c>
+      <c r="V15" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="W15" s="3">
+        <v>22100</v>
+      </c>
+      <c r="X15" s="3">
         <f t="shared" si="8"/>
-        <v>67.924528301886795</v>
-      </c>
-      <c r="U15" s="3">
-        <v>54900</v>
-      </c>
-      <c r="V15" s="3">
-        <v>1490000</v>
-      </c>
-      <c r="W15" s="3">
-        <v>10400</v>
-      </c>
-      <c r="X15" s="3">
+        <v>226.24434389140271</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>2877</v>
+      </c>
+      <c r="Z15" s="3">
         <f t="shared" si="9"/>
-        <v>143.26923076923077</v>
-      </c>
-      <c r="Y15" s="3">
-        <v>515</v>
-      </c>
-      <c r="Z15" s="3">
-        <f t="shared" si="10"/>
-        <v>331415</v>
+        <v>283277</v>
       </c>
       <c r="AA15" s="3">
+        <f t="shared" si="4"/>
+        <v>6560000</v>
+      </c>
+      <c r="AB15" s="3">
+        <f t="shared" si="4"/>
+        <v>57300</v>
+      </c>
+      <c r="AC15" s="3">
         <f t="shared" si="5"/>
-        <v>3290000</v>
-      </c>
-      <c r="AB15" s="3">
-        <f t="shared" si="5"/>
-        <v>36900</v>
-      </c>
-      <c r="AC15" s="3">
-        <f t="shared" si="11"/>
-        <v>89.159891598915991</v>
-      </c>
-      <c r="AD15" s="3">
-        <f t="shared" si="6"/>
-        <v>4159.8770746887967</v>
+        <v>5910.6835576923077</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
         <v>2</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E16">
-        <v>20220518</v>
+        <v>20220516</v>
       </c>
       <c r="F16">
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J16">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K16" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="L16" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="M16" t="s">
         <v>65</v>
       </c>
       <c r="N16" s="3">
-        <v>0</v>
+        <v>44500</v>
       </c>
       <c r="O16" s="3">
-        <v>9800000</v>
+        <v>12100000</v>
       </c>
       <c r="P16" s="3">
-        <v>113000</v>
+        <v>116000</v>
       </c>
       <c r="Q16" s="3">
+        <f t="shared" si="6"/>
+        <v>104.31034482758621</v>
+      </c>
+      <c r="R16" s="3">
+        <v>2260000</v>
+      </c>
+      <c r="S16" s="3">
+        <v>28100</v>
+      </c>
+      <c r="T16" s="3">
         <f t="shared" si="7"/>
-        <v>86.725663716814154</v>
-      </c>
-      <c r="R16" s="3">
-        <v>7050000</v>
-      </c>
-      <c r="S16" s="3">
-        <v>34500</v>
-      </c>
-      <c r="T16" s="3">
+        <v>80.42704626334519</v>
+      </c>
+      <c r="U16" s="3">
+        <v>46800</v>
+      </c>
+      <c r="V16" s="3">
+        <v>1100000</v>
+      </c>
+      <c r="W16" s="3">
+        <v>13300</v>
+      </c>
+      <c r="X16" s="3">
         <f t="shared" si="8"/>
-        <v>204.34782608695653</v>
-      </c>
-      <c r="U16" s="3">
-        <v>22600</v>
-      </c>
-      <c r="V16" s="3">
-        <v>485000</v>
-      </c>
-      <c r="W16" s="3">
-        <v>14700</v>
-      </c>
-      <c r="X16" s="3">
+        <v>82.706766917293237</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>1074</v>
+      </c>
+      <c r="Z16" s="3">
         <f t="shared" si="9"/>
-        <v>32.993197278911566</v>
-      </c>
-      <c r="Y16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="3">
-        <f t="shared" si="10"/>
-        <v>22600</v>
+        <v>92374</v>
       </c>
       <c r="AA16" s="3">
+        <f t="shared" si="4"/>
+        <v>3360000</v>
+      </c>
+      <c r="AB16" s="3">
+        <f t="shared" si="4"/>
+        <v>41400</v>
+      </c>
+      <c r="AC16" s="3">
         <f t="shared" si="5"/>
-        <v>7535000</v>
-      </c>
-      <c r="AB16" s="3">
-        <f t="shared" si="5"/>
-        <v>49200</v>
-      </c>
-      <c r="AC16" s="3">
-        <f t="shared" si="11"/>
-        <v>153.15040650406505</v>
-      </c>
-      <c r="AD16" s="3">
-        <f t="shared" si="6"/>
-        <v>260.59183673469391</v>
+        <v>885.56892561983466</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E17">
         <v>20220516</v>
@@ -3406,98 +3533,94 @@
         <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J17">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="K17" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="L17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="N17" s="3">
-        <v>249000</v>
+        <v>0</v>
       </c>
       <c r="O17" s="3">
-        <v>10400000</v>
+        <v>3280000</v>
       </c>
       <c r="P17" s="3">
-        <v>217000</v>
+        <v>57900</v>
       </c>
       <c r="Q17" s="3">
+        <f t="shared" si="6"/>
+        <v>56.649395509499136</v>
+      </c>
+      <c r="R17" s="3">
+        <v>178000</v>
+      </c>
+      <c r="S17" s="3">
+        <v>15700</v>
+      </c>
+      <c r="T17" s="3">
         <f t="shared" si="7"/>
-        <v>47.926267281105993</v>
-      </c>
-      <c r="R17" s="3">
-        <v>1560000</v>
-      </c>
-      <c r="S17" s="3">
-        <v>35200</v>
-      </c>
-      <c r="T17" s="3">
+        <v>11.337579617834395</v>
+      </c>
+      <c r="U17" s="3">
+        <v>8365</v>
+      </c>
+      <c r="V17" s="3">
+        <v>829000</v>
+      </c>
+      <c r="W17" s="3">
+        <v>14500</v>
+      </c>
+      <c r="X17" s="3">
         <f t="shared" si="8"/>
-        <v>44.31818181818182</v>
-      </c>
-      <c r="U17" s="3">
-        <v>31400</v>
-      </c>
-      <c r="V17" s="3">
-        <v>5000000</v>
-      </c>
-      <c r="W17" s="3">
-        <v>22100</v>
-      </c>
-      <c r="X17" s="3">
+        <v>57.172413793103445</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>1823</v>
+      </c>
+      <c r="Z17" s="3">
         <f t="shared" si="9"/>
-        <v>226.24434389140271</v>
-      </c>
-      <c r="Y17" s="3">
-        <v>2877</v>
-      </c>
-      <c r="Z17" s="3">
-        <f t="shared" si="10"/>
-        <v>283277</v>
+        <v>10188</v>
       </c>
       <c r="AA17" s="3">
+        <f t="shared" si="4"/>
+        <v>1007000</v>
+      </c>
+      <c r="AB17" s="3">
+        <f t="shared" si="4"/>
+        <v>30200</v>
+      </c>
+      <c r="AC17" s="3">
         <f t="shared" si="5"/>
-        <v>6560000</v>
-      </c>
-      <c r="AB17" s="3">
-        <f t="shared" si="5"/>
-        <v>57300</v>
-      </c>
-      <c r="AC17" s="3">
-        <f t="shared" si="11"/>
-        <v>114.48516579406632</v>
-      </c>
-      <c r="AD17" s="3">
-        <f t="shared" si="6"/>
-        <v>5910.6835576923077</v>
+        <v>179.84304878048781</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E18">
         <v>20220516</v>
@@ -3506,201 +3629,193 @@
         <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J18">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="K18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M18" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="N18" s="3">
-        <v>44500</v>
+        <v>5914</v>
       </c>
       <c r="O18" s="3">
-        <v>12100000</v>
+        <v>4380000</v>
       </c>
       <c r="P18" s="3">
-        <v>116000</v>
+        <v>56700</v>
       </c>
       <c r="Q18" s="3">
+        <f t="shared" si="6"/>
+        <v>77.248677248677254</v>
+      </c>
+      <c r="R18" s="3">
+        <v>1640000</v>
+      </c>
+      <c r="S18" s="3">
+        <v>22600</v>
+      </c>
+      <c r="T18" s="3">
         <f t="shared" si="7"/>
-        <v>104.31034482758621</v>
-      </c>
-      <c r="R18" s="3">
-        <v>2260000</v>
-      </c>
-      <c r="S18" s="3">
-        <v>28100</v>
-      </c>
-      <c r="T18" s="3">
+        <v>72.56637168141593</v>
+      </c>
+      <c r="U18" s="3">
+        <v>11100</v>
+      </c>
+      <c r="V18" s="3">
+        <v>1730000</v>
+      </c>
+      <c r="W18" s="3">
+        <v>12000</v>
+      </c>
+      <c r="X18" s="3">
         <f t="shared" si="8"/>
-        <v>80.42704626334519</v>
-      </c>
-      <c r="U18" s="3">
-        <v>46800</v>
-      </c>
-      <c r="V18" s="3">
-        <v>1100000</v>
-      </c>
-      <c r="W18" s="3">
-        <v>13300</v>
-      </c>
-      <c r="X18" s="3">
+        <v>144.16666666666666</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>11600</v>
+      </c>
+      <c r="Z18" s="3">
         <f t="shared" si="9"/>
-        <v>82.706766917293237</v>
-      </c>
-      <c r="Y18" s="3">
-        <v>1074</v>
-      </c>
-      <c r="Z18" s="3">
-        <f t="shared" si="10"/>
-        <v>92374</v>
+        <v>28614</v>
       </c>
       <c r="AA18" s="3">
+        <f t="shared" si="4"/>
+        <v>3370000</v>
+      </c>
+      <c r="AB18" s="3">
+        <f t="shared" si="4"/>
+        <v>34600</v>
+      </c>
+      <c r="AC18" s="3">
         <f t="shared" si="5"/>
-        <v>3360000</v>
-      </c>
-      <c r="AB18" s="3">
-        <f t="shared" si="5"/>
-        <v>41400</v>
-      </c>
-      <c r="AC18" s="3">
-        <f t="shared" si="11"/>
-        <v>81.159420289855078</v>
-      </c>
-      <c r="AD18" s="3">
-        <f t="shared" si="6"/>
-        <v>885.56892561983466</v>
+        <v>370.41410958904106</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E19">
-        <v>20220516</v>
+        <v>20220517</v>
       </c>
       <c r="F19">
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J19">
         <v>100</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="M19" t="s">
         <v>75</v>
       </c>
       <c r="N19" s="3">
-        <v>0</v>
+        <v>6976</v>
       </c>
       <c r="O19" s="3">
-        <v>3280000</v>
+        <v>1820000</v>
       </c>
       <c r="P19" s="3">
-        <v>57900</v>
+        <v>26900</v>
       </c>
       <c r="Q19" s="3">
+        <f t="shared" si="6"/>
+        <v>67.657992565055764</v>
+      </c>
+      <c r="R19" s="3">
+        <v>1690000</v>
+      </c>
+      <c r="S19" s="3">
+        <v>21500</v>
+      </c>
+      <c r="T19" s="3">
         <f t="shared" si="7"/>
-        <v>56.649395509499136</v>
-      </c>
-      <c r="R19" s="3">
-        <v>178000</v>
-      </c>
-      <c r="S19" s="3">
-        <v>15700</v>
-      </c>
-      <c r="T19" s="3">
-        <f t="shared" si="8"/>
-        <v>11.337579617834395</v>
+        <v>78.604651162790702</v>
       </c>
       <c r="U19" s="3">
-        <v>8365</v>
+        <v>15800</v>
       </c>
       <c r="V19" s="3">
-        <v>829000</v>
+        <v>1500000</v>
       </c>
       <c r="W19" s="3">
-        <v>14500</v>
+        <v>6035</v>
       </c>
       <c r="X19" s="3">
+        <f>V19/W19</f>
+        <v>248.55012427506213</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>1575</v>
+      </c>
+      <c r="Z19" s="3">
         <f t="shared" si="9"/>
-        <v>57.172413793103445</v>
-      </c>
-      <c r="Y19" s="3">
-        <v>1823</v>
-      </c>
-      <c r="Z19" s="3">
-        <f t="shared" si="10"/>
-        <v>10188</v>
+        <v>24351</v>
       </c>
       <c r="AA19" s="3">
+        <f t="shared" si="4"/>
+        <v>3190000</v>
+      </c>
+      <c r="AB19" s="3">
+        <f t="shared" si="4"/>
+        <v>27535</v>
+      </c>
+      <c r="AC19" s="3">
         <f t="shared" si="5"/>
-        <v>1007000</v>
-      </c>
-      <c r="AB19" s="3">
-        <f t="shared" si="5"/>
-        <v>30200</v>
-      </c>
-      <c r="AC19" s="3">
-        <f t="shared" si="11"/>
-        <v>33.34437086092715</v>
-      </c>
-      <c r="AD19" s="3">
-        <f t="shared" si="6"/>
-        <v>179.84304878048781</v>
+        <v>359.91313186813187</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
         <v>7</v>
       </c>
-      <c r="B20">
-        <v>6</v>
-      </c>
       <c r="C20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E20">
-        <v>20220516</v>
+        <v>20220517</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -3709,95 +3824,91 @@
         <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J20">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="K20" t="s">
         <v>77</v>
       </c>
       <c r="L20" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="M20" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="N20" s="3">
-        <v>5914</v>
+        <v>1197</v>
       </c>
       <c r="O20" s="3">
-        <v>4380000</v>
+        <v>20800000</v>
       </c>
       <c r="P20" s="3">
-        <v>56700</v>
+        <v>74700</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" si="7"/>
-        <v>77.248677248677254</v>
+        <f t="shared" si="6"/>
+        <v>278.44712182061579</v>
       </c>
       <c r="R20" s="3">
-        <v>1640000</v>
+        <v>3530000</v>
       </c>
       <c r="S20" s="3">
-        <v>22600</v>
+        <v>25200</v>
       </c>
       <c r="T20" s="3">
+        <f>R20/S20</f>
+        <v>140.07936507936509</v>
+      </c>
+      <c r="U20" s="3">
+        <v>6854</v>
+      </c>
+      <c r="V20" s="3">
+        <v>3540000</v>
+      </c>
+      <c r="W20" s="3">
+        <v>5493</v>
+      </c>
+      <c r="X20" s="3">
         <f t="shared" si="8"/>
-        <v>72.56637168141593</v>
-      </c>
-      <c r="U20" s="3">
-        <v>11100</v>
-      </c>
-      <c r="V20" s="3">
-        <v>1730000</v>
-      </c>
-      <c r="W20" s="3">
-        <v>12000</v>
-      </c>
-      <c r="X20" s="3">
+        <v>644.45658110322233</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
         <f t="shared" si="9"/>
-        <v>144.16666666666666</v>
-      </c>
-      <c r="Y20" s="3">
-        <v>11600</v>
-      </c>
-      <c r="Z20" s="3">
-        <f t="shared" si="10"/>
-        <v>28614</v>
+        <v>8051</v>
       </c>
       <c r="AA20" s="3">
+        <f t="shared" si="4"/>
+        <v>7070000</v>
+      </c>
+      <c r="AB20" s="3">
+        <f t="shared" si="4"/>
+        <v>30693</v>
+      </c>
+      <c r="AC20" s="3">
         <f t="shared" si="5"/>
-        <v>3370000</v>
-      </c>
-      <c r="AB20" s="3">
-        <f t="shared" si="5"/>
-        <v>34600</v>
-      </c>
-      <c r="AC20" s="3">
-        <f t="shared" si="11"/>
-        <v>97.398843930635834</v>
-      </c>
-      <c r="AD20" s="3">
-        <f t="shared" si="6"/>
-        <v>370.41410958904106</v>
+        <v>28.913927884615386</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E21">
         <v>20220517</v>
@@ -3806,89 +3917,85 @@
         <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J21">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="L21" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="M21" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="N21" s="3">
-        <v>6976</v>
+        <v>133000</v>
       </c>
       <c r="O21" s="3">
-        <v>1820000</v>
+        <v>1060000</v>
       </c>
       <c r="P21" s="3">
-        <v>26900</v>
+        <v>76400</v>
       </c>
       <c r="Q21" s="3">
+        <f t="shared" si="6"/>
+        <v>13.874345549738219</v>
+      </c>
+      <c r="R21" s="3">
+        <v>682000</v>
+      </c>
+      <c r="S21" s="3">
+        <v>15800</v>
+      </c>
+      <c r="T21" s="3">
         <f t="shared" si="7"/>
-        <v>67.657992565055764</v>
-      </c>
-      <c r="R21" s="3">
-        <v>1690000</v>
-      </c>
-      <c r="S21" s="3">
-        <v>21500</v>
-      </c>
-      <c r="T21" s="3">
+        <v>43.164556962025316</v>
+      </c>
+      <c r="U21" s="3">
+        <v>54800</v>
+      </c>
+      <c r="V21" s="3">
+        <v>455000</v>
+      </c>
+      <c r="W21" s="3">
+        <v>4172</v>
+      </c>
+      <c r="X21" s="3">
         <f t="shared" si="8"/>
-        <v>78.604651162790702</v>
-      </c>
-      <c r="U21" s="3">
-        <v>15800</v>
-      </c>
-      <c r="V21" s="3">
-        <v>1500000</v>
-      </c>
-      <c r="W21" s="3">
-        <v>6035</v>
-      </c>
-      <c r="X21" s="3">
-        <f>V21/W21</f>
-        <v>248.55012427506213</v>
+        <v>109.06040268456375</v>
       </c>
       <c r="Y21" s="3">
-        <v>1575</v>
+        <v>5359</v>
       </c>
       <c r="Z21" s="3">
-        <f t="shared" si="10"/>
-        <v>24351</v>
+        <f t="shared" si="9"/>
+        <v>193159</v>
       </c>
       <c r="AA21" s="3">
+        <f t="shared" si="4"/>
+        <v>1137000</v>
+      </c>
+      <c r="AB21" s="3">
+        <f t="shared" si="4"/>
+        <v>19972</v>
+      </c>
+      <c r="AC21" s="3">
         <f t="shared" si="5"/>
-        <v>3190000</v>
-      </c>
-      <c r="AB21" s="3">
-        <f t="shared" si="5"/>
-        <v>27535</v>
-      </c>
-      <c r="AC21" s="3">
-        <f t="shared" si="11"/>
-        <v>115.85255129834756</v>
-      </c>
-      <c r="AD21" s="3">
-        <f t="shared" si="6"/>
-        <v>359.91313186813187</v>
+        <v>13922.02603773585</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -3897,299 +4004,405 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="E22">
-        <v>20220517</v>
+        <v>20220524</v>
       </c>
       <c r="F22">
         <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J22">
         <v>100</v>
       </c>
       <c r="K22" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="L22" t="s">
-        <v>82</v>
-      </c>
-      <c r="M22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="N22" s="3">
-        <v>1197</v>
-      </c>
-      <c r="O22" s="3">
-        <v>20800000</v>
-      </c>
-      <c r="P22" s="3">
-        <v>74700</v>
-      </c>
-      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>1050000</v>
+      </c>
+      <c r="S22" s="3">
+        <v>37000</v>
+      </c>
+      <c r="T22" s="3">
         <f t="shared" si="7"/>
-        <v>278.44712182061579</v>
-      </c>
-      <c r="R22" s="3">
-        <v>3530000</v>
-      </c>
-      <c r="S22" s="3">
-        <v>25200</v>
-      </c>
-      <c r="T22" s="3">
-        <f>R22/S22</f>
-        <v>140.07936507936509</v>
+        <v>28.378378378378379</v>
       </c>
       <c r="U22" s="3">
-        <v>6854</v>
+        <v>0</v>
       </c>
       <c r="V22" s="3">
-        <v>3540000</v>
+        <v>192000</v>
       </c>
       <c r="W22" s="3">
-        <v>5493</v>
+        <v>13800</v>
       </c>
       <c r="X22" s="3">
-        <f t="shared" si="9"/>
-        <v>644.45658110322233</v>
+        <f t="shared" ref="X22:X31" si="10">V22/W22</f>
+        <v>13.913043478260869</v>
       </c>
       <c r="Y22" s="3">
         <v>0</v>
       </c>
       <c r="Z22" s="3">
-        <f t="shared" si="10"/>
-        <v>8051</v>
+        <f t="shared" ref="Z22:Z31" si="11">N22+U22+Y22</f>
+        <v>0</v>
       </c>
       <c r="AA22" s="3">
-        <f t="shared" si="5"/>
-        <v>7070000</v>
+        <f t="shared" si="4"/>
+        <v>1242000</v>
       </c>
       <c r="AB22" s="3">
-        <f t="shared" si="5"/>
-        <v>30693</v>
-      </c>
-      <c r="AC22" s="3">
-        <f t="shared" si="11"/>
-        <v>230.34568142573224</v>
-      </c>
-      <c r="AD22" s="3">
-        <f t="shared" si="6"/>
-        <v>28.913927884615386</v>
+        <f t="shared" si="4"/>
+        <v>50800</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B23">
         <v>7</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
         <v>84</v>
       </c>
       <c r="E23">
-        <v>20220517</v>
+        <v>20220524</v>
       </c>
       <c r="F23">
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J23">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="K23" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" t="s">
         <v>86</v>
       </c>
-      <c r="L23" t="s">
-        <v>87</v>
-      </c>
-      <c r="M23" t="s">
-        <v>63</v>
-      </c>
       <c r="N23" s="3">
-        <v>133000</v>
-      </c>
-      <c r="O23" s="3">
-        <v>1060000</v>
-      </c>
-      <c r="P23" s="3">
-        <v>76400</v>
-      </c>
-      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <v>710000</v>
+      </c>
+      <c r="S23" s="3">
+        <v>49900</v>
+      </c>
+      <c r="T23" s="3">
         <f t="shared" si="7"/>
-        <v>13.874345549738219</v>
-      </c>
-      <c r="R23" s="3">
-        <v>682000</v>
-      </c>
-      <c r="S23" s="3">
-        <v>15800</v>
-      </c>
-      <c r="T23" s="3">
-        <f t="shared" si="8"/>
-        <v>43.164556962025316</v>
+        <v>14.228456913827655</v>
       </c>
       <c r="U23" s="3">
-        <v>54800</v>
+        <v>0</v>
       </c>
       <c r="V23" s="3">
-        <v>455000</v>
+        <v>29000</v>
       </c>
       <c r="W23" s="3">
-        <v>4172</v>
+        <v>10300</v>
       </c>
       <c r="X23" s="3">
-        <f t="shared" si="9"/>
-        <v>109.06040268456375</v>
+        <f t="shared" si="10"/>
+        <v>2.8155339805825244</v>
       </c>
       <c r="Y23" s="3">
-        <v>5359</v>
+        <v>0</v>
       </c>
       <c r="Z23" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="3">
+        <f t="shared" si="4"/>
+        <v>739000</v>
+      </c>
+      <c r="AB23" s="3">
+        <f t="shared" si="4"/>
+        <v>60200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24">
+        <v>20220525</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" t="s">
+        <v>86</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0</v>
+      </c>
+      <c r="R24" s="3">
+        <v>950000</v>
+      </c>
+      <c r="S24" s="3">
+        <v>55300</v>
+      </c>
+      <c r="T24" s="3">
+        <f t="shared" si="7"/>
+        <v>17.179023508137433</v>
+      </c>
+      <c r="U24" s="3">
+        <v>0</v>
+      </c>
+      <c r="V24" s="3">
+        <v>722000</v>
+      </c>
+      <c r="W24" s="3">
+        <v>12700</v>
+      </c>
+      <c r="X24" s="3">
         <f t="shared" si="10"/>
-        <v>193159</v>
-      </c>
-      <c r="AA23" s="3">
-        <f t="shared" si="5"/>
-        <v>1137000</v>
-      </c>
-      <c r="AB23" s="3">
-        <f t="shared" si="5"/>
-        <v>19972</v>
-      </c>
-      <c r="AC23" s="3">
+        <v>56.8503937007874</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
         <f t="shared" si="11"/>
-        <v>56.929701582215102</v>
-      </c>
-      <c r="AD23" s="3">
-        <f t="shared" si="6"/>
-        <v>13922.02603773585</v>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="3">
+        <f t="shared" si="4"/>
+        <v>1672000</v>
+      </c>
+      <c r="AB24" s="3">
+        <f t="shared" si="4"/>
+        <v>68000</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="Z24" s="3">
-        <f>MEDIAN(Z14:Z23)</f>
-        <v>26482.5</v>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25">
+        <v>20220525</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" t="s">
+        <v>86</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0</v>
+      </c>
+      <c r="R25" s="3">
+        <v>53100</v>
+      </c>
+      <c r="S25" s="3">
+        <v>34600</v>
+      </c>
+      <c r="T25" s="3">
+        <f t="shared" si="7"/>
+        <v>1.5346820809248556</v>
+      </c>
+      <c r="U25" s="3">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3">
+        <v>71800</v>
+      </c>
+      <c r="W25" s="3">
+        <v>12100</v>
+      </c>
+      <c r="X25" s="3">
+        <f t="shared" si="10"/>
+        <v>5.9338842975206614</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="3">
+        <f t="shared" si="4"/>
+        <v>124900</v>
+      </c>
+      <c r="AB25" s="3">
+        <f t="shared" si="4"/>
+        <v>46700</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>7</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E26">
-        <v>20220524</v>
+        <v>20220526</v>
       </c>
       <c r="F26">
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J26">
         <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N26" s="3">
         <v>0</v>
       </c>
       <c r="R26" s="3">
-        <v>1050000</v>
+        <v>135000</v>
       </c>
       <c r="S26" s="3">
-        <v>37000</v>
+        <v>60400</v>
       </c>
       <c r="T26" s="3">
-        <f t="shared" si="8"/>
-        <v>28.378378378378379</v>
+        <f t="shared" si="7"/>
+        <v>2.2350993377483444</v>
       </c>
       <c r="U26" s="3">
         <v>0</v>
       </c>
       <c r="V26" s="3">
-        <v>192000</v>
+        <v>181000</v>
       </c>
       <c r="W26" s="3">
-        <v>13800</v>
+        <v>13200</v>
       </c>
       <c r="X26" s="3">
-        <f t="shared" ref="X26:X35" si="12">V26/W26</f>
-        <v>13.913043478260869</v>
+        <f t="shared" si="10"/>
+        <v>13.712121212121213</v>
       </c>
       <c r="Y26" s="3">
         <v>0</v>
       </c>
       <c r="Z26" s="3">
-        <f t="shared" ref="Z26:Z35" si="13">N26+U26+Y26</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA26" s="3">
-        <f t="shared" si="5"/>
-        <v>1242000</v>
+        <f t="shared" si="4"/>
+        <v>316000</v>
       </c>
       <c r="AB26" s="3">
-        <f t="shared" si="5"/>
-        <v>50800</v>
-      </c>
-      <c r="AC26" s="3">
-        <f t="shared" ref="AC26:AC35" si="14">AA26/AB26</f>
-        <v>24.448818897637796</v>
+        <f t="shared" si="4"/>
+        <v>73600</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B27">
         <v>7</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E27">
-        <v>20220524</v>
+        <v>20220526</v>
       </c>
       <c r="F27">
         <v>8</v>
@@ -4198,81 +4411,77 @@
         <v>91</v>
       </c>
       <c r="H27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J27">
         <v>100</v>
       </c>
       <c r="K27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N27" s="3">
         <v>0</v>
       </c>
       <c r="R27" s="3">
-        <v>710000</v>
+        <v>165000</v>
       </c>
       <c r="S27" s="3">
-        <v>49900</v>
+        <v>31600</v>
       </c>
       <c r="T27" s="3">
-        <f t="shared" si="8"/>
-        <v>14.228456913827655</v>
+        <f t="shared" si="7"/>
+        <v>5.2215189873417724</v>
       </c>
       <c r="U27" s="3">
         <v>0</v>
       </c>
       <c r="V27" s="3">
-        <v>29000</v>
+        <v>54300</v>
       </c>
       <c r="W27" s="3">
-        <v>10300</v>
+        <v>19300</v>
       </c>
       <c r="X27" s="3">
-        <f t="shared" si="12"/>
-        <v>2.8155339805825244</v>
+        <f t="shared" si="10"/>
+        <v>2.8134715025906734</v>
       </c>
       <c r="Y27" s="3">
         <v>0</v>
       </c>
       <c r="Z27" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA27" s="3">
-        <f t="shared" si="5"/>
-        <v>739000</v>
+        <f t="shared" si="4"/>
+        <v>219300</v>
       </c>
       <c r="AB27" s="3">
-        <f t="shared" si="5"/>
-        <v>60200</v>
-      </c>
-      <c r="AC27" s="3">
-        <f t="shared" si="14"/>
-        <v>12.275747508305647</v>
+        <f t="shared" si="4"/>
+        <v>50900</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B28">
         <v>7</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E28">
-        <v>20220525</v>
+        <v>20220526</v>
       </c>
       <c r="F28">
         <v>8</v>
@@ -4281,81 +4490,77 @@
         <v>92</v>
       </c>
       <c r="H28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J28">
         <v>100</v>
       </c>
       <c r="K28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N28" s="3">
         <v>0</v>
       </c>
       <c r="R28" s="3">
-        <v>950000</v>
+        <v>399000</v>
       </c>
       <c r="S28" s="3">
-        <v>55300</v>
+        <v>43200</v>
       </c>
       <c r="T28" s="3">
-        <f t="shared" si="8"/>
-        <v>17.179023508137433</v>
+        <f t="shared" si="7"/>
+        <v>9.2361111111111107</v>
       </c>
       <c r="U28" s="3">
         <v>0</v>
       </c>
       <c r="V28" s="3">
-        <v>722000</v>
+        <v>1051</v>
       </c>
       <c r="W28" s="3">
-        <v>12700</v>
+        <v>16600</v>
       </c>
       <c r="X28" s="3">
-        <f t="shared" si="12"/>
-        <v>56.8503937007874</v>
+        <f t="shared" si="10"/>
+        <v>6.3313253012048196E-2</v>
       </c>
       <c r="Y28" s="3">
         <v>0</v>
       </c>
       <c r="Z28" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA28" s="3">
-        <f t="shared" si="5"/>
-        <v>1672000</v>
+        <f t="shared" si="4"/>
+        <v>400051</v>
       </c>
       <c r="AB28" s="3">
-        <f t="shared" si="5"/>
-        <v>68000</v>
-      </c>
-      <c r="AC28" s="3">
-        <f t="shared" si="14"/>
-        <v>24.588235294117649</v>
+        <f t="shared" si="4"/>
+        <v>59800</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B29">
         <v>7</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E29">
-        <v>20220525</v>
+        <v>20220526</v>
       </c>
       <c r="F29">
         <v>8</v>
@@ -4364,81 +4569,77 @@
         <v>93</v>
       </c>
       <c r="H29" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J29">
         <v>100</v>
       </c>
       <c r="K29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N29" s="3">
         <v>0</v>
       </c>
       <c r="R29" s="3">
-        <v>53100</v>
+        <v>131000</v>
       </c>
       <c r="S29" s="3">
-        <v>34600</v>
+        <v>44400</v>
       </c>
       <c r="T29" s="3">
-        <f t="shared" si="8"/>
-        <v>1.5346820809248556</v>
+        <f t="shared" si="7"/>
+        <v>2.9504504504504503</v>
       </c>
       <c r="U29" s="3">
         <v>0</v>
       </c>
       <c r="V29" s="3">
-        <v>71800</v>
+        <v>49000</v>
       </c>
       <c r="W29" s="3">
-        <v>12100</v>
+        <v>16300</v>
       </c>
       <c r="X29" s="3">
-        <f t="shared" si="12"/>
-        <v>5.9338842975206614</v>
+        <f t="shared" si="10"/>
+        <v>3.0061349693251533</v>
       </c>
       <c r="Y29" s="3">
         <v>0</v>
       </c>
       <c r="Z29" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA29" s="3">
-        <f t="shared" si="5"/>
-        <v>124900</v>
+        <f t="shared" si="4"/>
+        <v>180000</v>
       </c>
       <c r="AB29" s="3">
-        <f t="shared" si="5"/>
-        <v>46700</v>
-      </c>
-      <c r="AC29" s="3">
-        <f t="shared" si="14"/>
-        <v>2.6745182012847968</v>
+        <f t="shared" si="4"/>
+        <v>60700</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E30">
-        <v>20220526</v>
+        <v>20220531</v>
       </c>
       <c r="F30">
         <v>8</v>
@@ -4447,81 +4648,77 @@
         <v>94</v>
       </c>
       <c r="H30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N30" s="3">
         <v>0</v>
       </c>
       <c r="R30" s="3">
-        <v>135000</v>
+        <v>2270000</v>
       </c>
       <c r="S30" s="3">
-        <v>60400</v>
+        <v>47300</v>
       </c>
       <c r="T30" s="3">
-        <f t="shared" si="8"/>
-        <v>2.2350993377483444</v>
+        <f t="shared" si="7"/>
+        <v>47.991543340380552</v>
       </c>
       <c r="U30" s="3">
         <v>0</v>
       </c>
       <c r="V30" s="3">
-        <v>181000</v>
+        <v>165000</v>
       </c>
       <c r="W30" s="3">
-        <v>13200</v>
+        <v>17300</v>
       </c>
       <c r="X30" s="3">
-        <f t="shared" si="12"/>
-        <v>13.712121212121213</v>
+        <f t="shared" si="10"/>
+        <v>9.5375722543352595</v>
       </c>
       <c r="Y30" s="3">
         <v>0</v>
       </c>
       <c r="Z30" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA30" s="3">
-        <f t="shared" si="5"/>
-        <v>316000</v>
+        <f t="shared" si="4"/>
+        <v>2435000</v>
       </c>
       <c r="AB30" s="3">
-        <f t="shared" si="5"/>
-        <v>73600</v>
-      </c>
-      <c r="AC30" s="3">
-        <f t="shared" si="14"/>
-        <v>4.2934782608695654</v>
+        <f t="shared" si="4"/>
+        <v>64600</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E31">
-        <v>20220526</v>
+        <v>20220531</v>
       </c>
       <c r="F31">
         <v>8</v>
@@ -4530,396 +4727,60 @@
         <v>95</v>
       </c>
       <c r="H31" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J31">
         <v>100</v>
       </c>
       <c r="K31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L31" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N31" s="3">
         <v>0</v>
       </c>
       <c r="R31" s="3">
-        <v>165000</v>
+        <v>3710000</v>
       </c>
       <c r="S31" s="3">
-        <v>31600</v>
+        <v>45300</v>
       </c>
       <c r="T31" s="3">
-        <f t="shared" si="8"/>
-        <v>5.2215189873417724</v>
+        <f t="shared" si="7"/>
+        <v>81.898454746136863</v>
       </c>
       <c r="U31" s="3">
         <v>0</v>
       </c>
       <c r="V31" s="3">
-        <v>54300</v>
+        <v>168000</v>
       </c>
       <c r="W31" s="3">
-        <v>19300</v>
+        <v>17200</v>
       </c>
       <c r="X31" s="3">
-        <f t="shared" si="12"/>
-        <v>2.8134715025906734</v>
+        <f t="shared" si="10"/>
+        <v>9.7674418604651159</v>
       </c>
       <c r="Y31" s="3">
         <v>0</v>
       </c>
       <c r="Z31" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA31" s="3">
-        <f t="shared" si="5"/>
-        <v>219300</v>
+        <f t="shared" si="4"/>
+        <v>3878000</v>
       </c>
       <c r="AB31" s="3">
-        <f t="shared" si="5"/>
-        <v>50900</v>
-      </c>
-      <c r="AC31" s="3">
-        <f t="shared" si="14"/>
-        <v>4.3084479371316302</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="A32">
-        <v>7</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32">
-        <v>20220526</v>
-      </c>
-      <c r="F32">
-        <v>8</v>
-      </c>
-      <c r="G32" t="s">
-        <v>96</v>
-      </c>
-      <c r="H32" t="s">
-        <v>32</v>
-      </c>
-      <c r="I32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32">
-        <v>100</v>
-      </c>
-      <c r="K32" t="s">
-        <v>34</v>
-      </c>
-      <c r="L32" t="s">
-        <v>90</v>
-      </c>
-      <c r="N32" s="3">
-        <v>0</v>
-      </c>
-      <c r="R32" s="3">
-        <v>399000</v>
-      </c>
-      <c r="S32" s="3">
-        <v>43200</v>
-      </c>
-      <c r="T32" s="3">
-        <f t="shared" si="8"/>
-        <v>9.2361111111111107</v>
-      </c>
-      <c r="U32" s="3">
-        <v>0</v>
-      </c>
-      <c r="V32" s="3">
-        <v>1051</v>
-      </c>
-      <c r="W32" s="3">
-        <v>16600</v>
-      </c>
-      <c r="X32" s="3">
-        <f t="shared" si="12"/>
-        <v>6.3313253012048196E-2</v>
-      </c>
-      <c r="Y32" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AA32" s="3">
-        <f t="shared" si="5"/>
-        <v>400051</v>
-      </c>
-      <c r="AB32" s="3">
-        <f t="shared" si="5"/>
-        <v>59800</v>
-      </c>
-      <c r="AC32" s="3">
-        <f t="shared" si="14"/>
-        <v>6.6898160535117057</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A33">
-        <v>8</v>
-      </c>
-      <c r="B33">
-        <v>7</v>
-      </c>
-      <c r="C33">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33">
-        <v>20220526</v>
-      </c>
-      <c r="F33">
-        <v>8</v>
-      </c>
-      <c r="G33" t="s">
-        <v>97</v>
-      </c>
-      <c r="H33" t="s">
-        <v>32</v>
-      </c>
-      <c r="I33" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33">
-        <v>100</v>
-      </c>
-      <c r="K33" t="s">
-        <v>34</v>
-      </c>
-      <c r="L33" t="s">
-        <v>90</v>
-      </c>
-      <c r="N33" s="3">
-        <v>0</v>
-      </c>
-      <c r="R33" s="3">
-        <v>131000</v>
-      </c>
-      <c r="S33" s="3">
-        <v>44400</v>
-      </c>
-      <c r="T33" s="3">
-        <f t="shared" si="8"/>
-        <v>2.9504504504504503</v>
-      </c>
-      <c r="U33" s="3">
-        <v>0</v>
-      </c>
-      <c r="V33" s="3">
-        <v>49000</v>
-      </c>
-      <c r="W33" s="3">
-        <v>16300</v>
-      </c>
-      <c r="X33" s="3">
-        <f t="shared" si="12"/>
-        <v>3.0061349693251533</v>
-      </c>
-      <c r="Y33" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AA33" s="3">
-        <f t="shared" si="5"/>
-        <v>180000</v>
-      </c>
-      <c r="AB33" s="3">
-        <f t="shared" si="5"/>
-        <v>60700</v>
-      </c>
-      <c r="AC33" s="3">
-        <f t="shared" si="14"/>
-        <v>2.9654036243822075</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A34">
-        <v>9</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34">
-        <v>20220531</v>
-      </c>
-      <c r="F34">
-        <v>8</v>
-      </c>
-      <c r="G34" t="s">
-        <v>98</v>
-      </c>
-      <c r="H34" t="s">
-        <v>32</v>
-      </c>
-      <c r="I34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J34">
-        <v>100</v>
-      </c>
-      <c r="K34" t="s">
-        <v>34</v>
-      </c>
-      <c r="L34" t="s">
-        <v>90</v>
-      </c>
-      <c r="N34" s="3">
-        <v>0</v>
-      </c>
-      <c r="R34" s="3">
-        <v>2270000</v>
-      </c>
-      <c r="S34" s="3">
-        <v>47300</v>
-      </c>
-      <c r="T34" s="3">
-        <f t="shared" si="8"/>
-        <v>47.991543340380552</v>
-      </c>
-      <c r="U34" s="3">
-        <v>0</v>
-      </c>
-      <c r="V34" s="3">
-        <v>165000</v>
-      </c>
-      <c r="W34" s="3">
-        <v>17300</v>
-      </c>
-      <c r="X34" s="3">
-        <f t="shared" si="12"/>
-        <v>9.5375722543352595</v>
-      </c>
-      <c r="Y34" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AA34" s="3">
-        <f t="shared" si="5"/>
-        <v>2435000</v>
-      </c>
-      <c r="AB34" s="3">
-        <f t="shared" si="5"/>
-        <v>64600</v>
-      </c>
-      <c r="AC34" s="3">
-        <f t="shared" si="14"/>
-        <v>37.693498452012385</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A35">
-        <v>10</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35">
-        <v>20220531</v>
-      </c>
-      <c r="F35">
-        <v>8</v>
-      </c>
-      <c r="G35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I35" t="s">
-        <v>33</v>
-      </c>
-      <c r="J35">
-        <v>100</v>
-      </c>
-      <c r="K35" t="s">
-        <v>34</v>
-      </c>
-      <c r="L35" t="s">
-        <v>90</v>
-      </c>
-      <c r="N35" s="3">
-        <v>0</v>
-      </c>
-      <c r="R35" s="3">
-        <v>3710000</v>
-      </c>
-      <c r="S35" s="3">
-        <v>45300</v>
-      </c>
-      <c r="T35" s="3">
-        <f t="shared" si="8"/>
-        <v>81.898454746136863</v>
-      </c>
-      <c r="U35" s="3">
-        <v>0</v>
-      </c>
-      <c r="V35" s="3">
-        <v>168000</v>
-      </c>
-      <c r="W35" s="3">
-        <v>17200</v>
-      </c>
-      <c r="X35" s="3">
-        <f t="shared" si="12"/>
-        <v>9.7674418604651159</v>
-      </c>
-      <c r="Y35" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z35" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AA35" s="3">
-        <f t="shared" si="5"/>
-        <v>3878000</v>
-      </c>
-      <c r="AB35" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>62500</v>
-      </c>
-      <c r="AC35" s="3">
-        <f t="shared" si="14"/>
-        <v>62.048000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>